<commit_message>
Perbaikan Form Kwitansi V1
Sudah selesai
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyData\Github\simbaper\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7961CB-AB12-4D47-9C98-69BA6FFB9B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077F4A9F-EEB7-4A22-A93D-F12BFCDD6681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6670,9 +6670,6 @@
     <t>SWALLOW TWIN BALL 2 S 150 gr</t>
   </si>
   <si>
-    <t xml:space="preserve">      Nama :</t>
-  </si>
-  <si>
     <t>BADAN PUSAT STATISTIK</t>
   </si>
   <si>
@@ -6683,6 +6680,9 @@
   </si>
   <si>
     <t>NIP. 19810062006041008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Tim Kerja :</t>
   </si>
 </sst>
 </file>
@@ -8048,7 +8048,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="1"/>
     <xf numFmtId="41" fontId="31" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="362">
+  <cellXfs count="348">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -8711,9 +8711,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="37" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -8734,7 +8743,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1"/>
@@ -8744,8 +8759,11 @@
     <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8957,64 +8975,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -34771,13 +34731,13 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G11" sqref="G11:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.36328125" style="65" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" style="65" customWidth="1"/>
+    <col min="2" max="2" width="7.90625" style="65" customWidth="1"/>
     <col min="3" max="3" width="34.1796875" style="65" customWidth="1"/>
     <col min="4" max="5" width="9.36328125" style="65" customWidth="1"/>
     <col min="6" max="6" width="10.90625" style="65" bestFit="1" customWidth="1"/>
@@ -34799,24 +34759,24 @@
       <c r="G1" s="64"/>
     </row>
     <row r="2" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A2" s="255"/>
-      <c r="B2" s="255"/>
-      <c r="C2" s="261" t="s">
-        <v>2182</v>
-      </c>
-      <c r="D2" s="261"/>
-      <c r="E2" s="261"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="257"/>
+      <c r="C2" s="264" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D2" s="264"/>
+      <c r="E2" s="264"/>
       <c r="F2" s="64"/>
       <c r="G2" s="64"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="255"/>
-      <c r="B3" s="255"/>
-      <c r="C3" s="257" t="s">
-        <v>2183</v>
-      </c>
-      <c r="D3" s="257"/>
-      <c r="E3" s="257"/>
+      <c r="A3" s="257"/>
+      <c r="B3" s="257"/>
+      <c r="C3" s="260" t="s">
+        <v>2182</v>
+      </c>
+      <c r="D3" s="260"/>
+      <c r="E3" s="260"/>
       <c r="F3" s="67"/>
       <c r="G3" s="97"/>
     </row>
@@ -34839,106 +34799,106 @@
       <c r="G5" s="97"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="347"/>
-      <c r="B6" s="343"/>
-      <c r="C6" s="343"/>
-      <c r="D6" s="343"/>
-      <c r="E6" s="344"/>
-      <c r="F6" s="344"/>
-      <c r="G6" s="343"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="97"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="97"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="342" t="s">
+      <c r="A7" s="268" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="342"/>
-      <c r="C7" s="342"/>
-      <c r="D7" s="342"/>
-      <c r="E7" s="342"/>
-      <c r="F7" s="342"/>
-      <c r="G7" s="342"/>
+      <c r="B7" s="268"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="268"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="347"/>
-      <c r="B8" s="343"/>
-      <c r="C8" s="343"/>
-      <c r="D8" s="344"/>
-      <c r="E8" s="343"/>
-      <c r="F8" s="343"/>
-      <c r="G8" s="343"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="345" t="s">
-        <v>2181</v>
-      </c>
-      <c r="B9" s="345"/>
-      <c r="C9" s="346"/>
-      <c r="D9" s="346"/>
-      <c r="E9" s="343"/>
-      <c r="F9" s="343" t="s">
+      <c r="A9" s="263" t="s">
+        <v>2185</v>
+      </c>
+      <c r="B9" s="263"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="343"/>
+      <c r="G9" s="97"/>
     </row>
     <row r="10" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="347"/>
-      <c r="B10" s="343"/>
-      <c r="C10" s="343"/>
-      <c r="D10" s="344"/>
-      <c r="E10" s="343"/>
-      <c r="F10" s="345" t="s">
+      <c r="A10" s="96"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="263" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="345"/>
+      <c r="G10" s="263"/>
     </row>
     <row r="11" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="258" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="263" t="s">
+      <c r="B11" s="259" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="263"/>
-      <c r="D11" s="256" t="s">
+      <c r="C11" s="259"/>
+      <c r="D11" s="258" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="264"/>
-      <c r="F11" s="256" t="s">
+      <c r="E11" s="269"/>
+      <c r="F11" s="258" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="256" t="s">
+      <c r="G11" s="258" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="256"/>
-      <c r="B12" s="263"/>
-      <c r="C12" s="263"/>
-      <c r="D12" s="256" t="s">
+      <c r="A12" s="258"/>
+      <c r="B12" s="259"/>
+      <c r="C12" s="259"/>
+      <c r="D12" s="258" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="256" t="s">
+      <c r="E12" s="258" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="256"/>
-      <c r="G12" s="256"/>
+      <c r="F12" s="258"/>
+      <c r="G12" s="258"/>
     </row>
     <row r="13" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="256"/>
-      <c r="B13" s="263"/>
-      <c r="C13" s="263"/>
-      <c r="D13" s="265"/>
-      <c r="E13" s="265"/>
-      <c r="F13" s="256"/>
-      <c r="G13" s="256"/>
+      <c r="A13" s="258"/>
+      <c r="B13" s="259"/>
+      <c r="C13" s="259"/>
+      <c r="D13" s="270"/>
+      <c r="E13" s="270"/>
+      <c r="F13" s="258"/>
+      <c r="G13" s="258"/>
     </row>
     <row r="14" spans="1:7" s="243" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="251" t="str">
         <f>IF($B14&lt;&gt;"",COUNTA($B$14:$B14),"")</f>
         <v/>
       </c>
-      <c r="B14" s="259"/>
-      <c r="C14" s="259"/>
+      <c r="B14" s="262"/>
+      <c r="C14" s="262"/>
       <c r="D14" s="252"/>
       <c r="E14" s="252"/>
       <c r="F14" s="251"/>
@@ -34949,8 +34909,8 @@
         <f>IF($B15&lt;&gt;"",COUNTA($B$14:$B15),"")</f>
         <v/>
       </c>
-      <c r="B15" s="259"/>
-      <c r="C15" s="259"/>
+      <c r="B15" s="262"/>
+      <c r="C15" s="262"/>
       <c r="D15" s="252"/>
       <c r="E15" s="252"/>
       <c r="F15" s="251" t="str">
@@ -34964,8 +34924,8 @@
         <f>IF($B16&lt;&gt;"",COUNTA($B$14:$B16),"")</f>
         <v/>
       </c>
-      <c r="B16" s="259"/>
-      <c r="C16" s="259"/>
+      <c r="B16" s="262"/>
+      <c r="C16" s="262"/>
       <c r="D16" s="252"/>
       <c r="E16" s="252"/>
       <c r="F16" s="251" t="str">
@@ -34979,8 +34939,8 @@
         <f>IF($B17&lt;&gt;"",COUNTA($B$14:$B17),"")</f>
         <v/>
       </c>
-      <c r="B17" s="259"/>
-      <c r="C17" s="259"/>
+      <c r="B17" s="262"/>
+      <c r="C17" s="262"/>
       <c r="D17" s="252"/>
       <c r="E17" s="252"/>
       <c r="F17" s="251" t="str">
@@ -34994,8 +34954,8 @@
         <f>IF($B18&lt;&gt;"",COUNTA($B$14:$B18),"")</f>
         <v/>
       </c>
-      <c r="B18" s="259"/>
-      <c r="C18" s="259"/>
+      <c r="B18" s="262"/>
+      <c r="C18" s="262"/>
       <c r="D18" s="252"/>
       <c r="E18" s="252"/>
       <c r="F18" s="251" t="str">
@@ -35009,8 +34969,8 @@
         <f>IF($B19&lt;&gt;"",COUNTA($B$14:$B19),"")</f>
         <v/>
       </c>
-      <c r="B19" s="259"/>
-      <c r="C19" s="259"/>
+      <c r="B19" s="262"/>
+      <c r="C19" s="262"/>
       <c r="D19" s="252"/>
       <c r="E19" s="252"/>
       <c r="F19" s="251" t="str">
@@ -35024,8 +34984,8 @@
         <f>IF($B20&lt;&gt;"",COUNTA($B$14:$B20),"")</f>
         <v/>
       </c>
-      <c r="B20" s="259"/>
-      <c r="C20" s="259"/>
+      <c r="B20" s="262"/>
+      <c r="C20" s="262"/>
       <c r="D20" s="252"/>
       <c r="E20" s="252"/>
       <c r="F20" s="251" t="str">
@@ -35039,8 +34999,8 @@
         <f>IF($B21&lt;&gt;"",COUNTA($B$14:$B21),"")</f>
         <v/>
       </c>
-      <c r="B21" s="259"/>
-      <c r="C21" s="259"/>
+      <c r="B21" s="262"/>
+      <c r="C21" s="262"/>
       <c r="D21" s="252"/>
       <c r="E21" s="252" t="str">
         <f t="shared" ref="E21:E26" si="0">IF($D21&lt;&gt;"",D21,"")</f>
@@ -35054,8 +35014,8 @@
         <f>IF($B22&lt;&gt;"",COUNTA($B$14:$B22),"")</f>
         <v/>
       </c>
-      <c r="B22" s="259"/>
-      <c r="C22" s="259"/>
+      <c r="B22" s="262"/>
+      <c r="C22" s="262"/>
       <c r="D22" s="252"/>
       <c r="E22" s="252" t="str">
         <f t="shared" si="0"/>
@@ -35072,8 +35032,8 @@
         <f>IF($B23&lt;&gt;"",COUNTA($B$14:$B23),"")</f>
         <v/>
       </c>
-      <c r="B23" s="259"/>
-      <c r="C23" s="259"/>
+      <c r="B23" s="262"/>
+      <c r="C23" s="262"/>
       <c r="D23" s="252"/>
       <c r="E23" s="252" t="str">
         <f t="shared" si="0"/>
@@ -35090,8 +35050,8 @@
         <f>IF($B24&lt;&gt;"",COUNTA($B$14:$B24),"")</f>
         <v/>
       </c>
-      <c r="B24" s="259"/>
-      <c r="C24" s="259"/>
+      <c r="B24" s="262"/>
+      <c r="C24" s="262"/>
       <c r="D24" s="252"/>
       <c r="E24" s="252" t="str">
         <f t="shared" si="0"/>
@@ -35108,8 +35068,8 @@
         <f>IF($B25&lt;&gt;"",COUNTA($B$14:$B25),"")</f>
         <v/>
       </c>
-      <c r="B25" s="259"/>
-      <c r="C25" s="259"/>
+      <c r="B25" s="262"/>
+      <c r="C25" s="262"/>
       <c r="D25" s="252"/>
       <c r="E25" s="252" t="str">
         <f t="shared" si="0"/>
@@ -35126,8 +35086,8 @@
         <f>IF($B26&lt;&gt;"",COUNTA($B$14:$B26),"")</f>
         <v/>
       </c>
-      <c r="B26" s="259"/>
-      <c r="C26" s="259"/>
+      <c r="B26" s="262"/>
+      <c r="C26" s="262"/>
       <c r="D26" s="252"/>
       <c r="E26" s="252" t="str">
         <f t="shared" si="0"/>
@@ -35144,8 +35104,8 @@
         <f>IF($B27&lt;&gt;"",COUNTA($B$14:$B27),"")</f>
         <v/>
       </c>
-      <c r="B27" s="259"/>
-      <c r="C27" s="259"/>
+      <c r="B27" s="262"/>
+      <c r="C27" s="262"/>
       <c r="D27" s="252"/>
       <c r="E27" s="252" t="str">
         <f t="shared" ref="E27" si="1">IF($D27&lt;&gt;"",D27,"")</f>
@@ -35158,114 +35118,106 @@
       <c r="G27" s="254"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="347"/>
-      <c r="B28" s="343"/>
-      <c r="C28" s="343"/>
-      <c r="D28" s="348"/>
-      <c r="E28" s="343"/>
-      <c r="F28" s="343"/>
-      <c r="G28" s="343"/>
+      <c r="A28" s="96"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="347"/>
-      <c r="B29" s="343"/>
-      <c r="C29" s="343"/>
-      <c r="D29" s="343"/>
-      <c r="E29" s="349"/>
-      <c r="F29" s="343"/>
-      <c r="G29" s="343"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="97"/>
+      <c r="G29" s="97"/>
       <c r="H29" s="249"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="347"/>
-      <c r="B30" s="349"/>
-      <c r="C30" s="343"/>
-      <c r="D30" s="350"/>
-      <c r="E30" s="351"/>
-      <c r="F30" s="351"/>
-      <c r="G30" s="351"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="271"/>
+      <c r="F30" s="271"/>
+      <c r="G30" s="271"/>
       <c r="H30" s="250"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="352"/>
-      <c r="B31" s="353" t="s">
+      <c r="B31" s="272" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="353"/>
-      <c r="D31" s="344"/>
-      <c r="E31" s="354" t="s">
+      <c r="C31" s="272"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="267" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="354"/>
-      <c r="G31" s="354"/>
+      <c r="F31" s="267"/>
+      <c r="G31" s="267"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="352"/>
-      <c r="B32" s="355"/>
-      <c r="C32" s="356"/>
-      <c r="D32" s="344"/>
-      <c r="E32" s="343"/>
-      <c r="F32" s="343"/>
-      <c r="G32" s="343"/>
+      <c r="B32" s="255"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="352"/>
-      <c r="B33" s="355"/>
-      <c r="C33" s="356"/>
-      <c r="D33" s="344"/>
-      <c r="E33" s="343"/>
-      <c r="F33" s="343"/>
-      <c r="G33" s="343"/>
+      <c r="B33" s="255"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="97"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="352"/>
-      <c r="B34" s="355"/>
-      <c r="C34" s="356"/>
-      <c r="D34" s="344"/>
-      <c r="E34" s="343"/>
-      <c r="F34" s="343"/>
-      <c r="G34" s="343"/>
+      <c r="B34" s="255"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="352"/>
-      <c r="B35" s="357" t="s">
+      <c r="B35" s="273" t="s">
+        <v>2183</v>
+      </c>
+      <c r="C35" s="273"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="265"/>
+      <c r="F35" s="265"/>
+      <c r="G35" s="265"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="257" t="s">
         <v>2184</v>
       </c>
-      <c r="C35" s="357"/>
-      <c r="D35" s="344"/>
-      <c r="E35" s="358"/>
-      <c r="F35" s="358"/>
-      <c r="G35" s="358"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="352"/>
-      <c r="B36" s="359" t="s">
-        <v>2185</v>
-      </c>
-      <c r="C36" s="359"/>
-      <c r="D36" s="344"/>
-      <c r="E36" s="354"/>
-      <c r="F36" s="354"/>
-      <c r="G36" s="354"/>
+      <c r="C36" s="257"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="267"/>
+      <c r="F36" s="267"/>
+      <c r="G36" s="267"/>
     </row>
     <row r="37" spans="1:7" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="352"/>
-      <c r="B37" s="352"/>
-      <c r="C37" s="360"/>
-      <c r="D37" s="348"/>
-      <c r="E37" s="361" t="str">
+      <c r="C37" s="256"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="266" t="str">
         <f>_xlfn.XLOOKUP($E36,db_pegawai!$B$2:$B$90,db_pegawai!$I$2:$I$90,"")</f>
         <v/>
       </c>
-      <c r="F37" s="354"/>
-      <c r="G37" s="354"/>
+      <c r="F37" s="267"/>
+      <c r="G37" s="267"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="258" t="s">
+      <c r="A38" s="261" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="258"/>
-      <c r="C38" s="258"/>
+      <c r="B38" s="261"/>
+      <c r="C38" s="261"/>
       <c r="D38" s="64"/>
       <c r="E38" s="64"/>
       <c r="F38" s="64"/>
@@ -35273,20 +35225,10 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="A11:A13"/>
@@ -35302,13 +35244,23 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="E35:G35"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E37:G37"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="B11:C13"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.98425196850393704" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
@@ -35595,15 +35547,15 @@
       <c r="G6" s="100"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="301" t="s">
+      <c r="A7" s="307" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="302"/>
-      <c r="C7" s="302"/>
-      <c r="D7" s="302"/>
-      <c r="E7" s="302"/>
-      <c r="F7" s="302"/>
-      <c r="G7" s="303"/>
+      <c r="B7" s="308"/>
+      <c r="C7" s="308"/>
+      <c r="D7" s="308"/>
+      <c r="E7" s="308"/>
+      <c r="F7" s="308"/>
+      <c r="G7" s="309"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="101"/>
@@ -35615,10 +35567,10 @@
       <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="304" t="s">
+      <c r="A9" s="310" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="260"/>
+      <c r="B9" s="263"/>
       <c r="C9" s="103" t="str">
         <f>_xlfn.XLOOKUP($E35,Table5[Nama pegawai],Table5[Ruangan],"")</f>
         <v/>
@@ -35645,10 +35597,10 @@
       <c r="A11" s="107"/>
       <c r="B11" s="71"/>
       <c r="C11" s="69"/>
-      <c r="D11" s="305" t="s">
+      <c r="D11" s="311" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="306"/>
+      <c r="E11" s="312"/>
       <c r="F11" s="108"/>
       <c r="G11" s="109"/>
     </row>
@@ -35656,14 +35608,14 @@
       <c r="A12" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="307" t="s">
+      <c r="B12" s="313" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="308"/>
-      <c r="D12" s="309" t="s">
+      <c r="C12" s="314"/>
+      <c r="D12" s="315" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="309" t="s">
+      <c r="E12" s="315" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="111" t="s">
@@ -35677,8 +35629,8 @@
       <c r="A13" s="113"/>
       <c r="B13" s="83"/>
       <c r="C13" s="84"/>
-      <c r="D13" s="310"/>
-      <c r="E13" s="310"/>
+      <c r="D13" s="316"/>
+      <c r="E13" s="316"/>
       <c r="F13" s="114"/>
       <c r="G13" s="115"/>
     </row>
@@ -35687,8 +35639,8 @@
         <f>IF($B14&lt;&gt;"",COUNTA($B$14:$B14),"")</f>
         <v/>
       </c>
-      <c r="B14" s="311"/>
-      <c r="C14" s="311"/>
+      <c r="B14" s="317"/>
+      <c r="C14" s="317"/>
       <c r="D14" s="117"/>
       <c r="E14" s="117"/>
       <c r="F14" s="118" t="str">
@@ -35702,8 +35654,8 @@
         <f>IF($B15&lt;&gt;"",COUNTA($B$14:$B15),"")</f>
         <v/>
       </c>
-      <c r="B15" s="300"/>
-      <c r="C15" s="300"/>
+      <c r="B15" s="306"/>
+      <c r="C15" s="306"/>
       <c r="D15" s="121"/>
       <c r="E15" s="121"/>
       <c r="F15" s="122" t="str">
@@ -35717,8 +35669,8 @@
         <f>IF($B16&lt;&gt;"",COUNTA($B$14:$B16),"")</f>
         <v/>
       </c>
-      <c r="B16" s="300"/>
-      <c r="C16" s="300"/>
+      <c r="B16" s="306"/>
+      <c r="C16" s="306"/>
       <c r="D16" s="121"/>
       <c r="E16" s="121" t="str">
         <f t="shared" ref="E16:E27" si="0">IF($D16&lt;&gt;"",D16,"")</f>
@@ -35735,8 +35687,8 @@
         <f>IF($B17&lt;&gt;"",COUNTA($B$14:$B17),"")</f>
         <v/>
       </c>
-      <c r="B17" s="300"/>
-      <c r="C17" s="300"/>
+      <c r="B17" s="306"/>
+      <c r="C17" s="306"/>
       <c r="D17" s="124"/>
       <c r="E17" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35753,8 +35705,8 @@
         <f>IF($B18&lt;&gt;"",COUNTA($B$14:$B18),"")</f>
         <v/>
       </c>
-      <c r="B18" s="300"/>
-      <c r="C18" s="300"/>
+      <c r="B18" s="306"/>
+      <c r="C18" s="306"/>
       <c r="D18" s="126"/>
       <c r="E18" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35771,8 +35723,8 @@
         <f>IF($B19&lt;&gt;"",COUNTA($B$14:$B19),"")</f>
         <v/>
       </c>
-      <c r="B19" s="300"/>
-      <c r="C19" s="300"/>
+      <c r="B19" s="306"/>
+      <c r="C19" s="306"/>
       <c r="D19" s="126"/>
       <c r="E19" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35789,8 +35741,8 @@
         <f>IF($B20&lt;&gt;"",COUNTA($B$14:$B20),"")</f>
         <v/>
       </c>
-      <c r="B20" s="300"/>
-      <c r="C20" s="300"/>
+      <c r="B20" s="306"/>
+      <c r="C20" s="306"/>
       <c r="D20" s="126"/>
       <c r="E20" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35807,8 +35759,8 @@
         <f>IF($B21&lt;&gt;"",COUNTA($B$14:$B21),"")</f>
         <v/>
       </c>
-      <c r="B21" s="300"/>
-      <c r="C21" s="300"/>
+      <c r="B21" s="306"/>
+      <c r="C21" s="306"/>
       <c r="D21" s="126"/>
       <c r="E21" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35825,8 +35777,8 @@
         <f>IF($B22&lt;&gt;"",COUNTA($B$14:$B22),"")</f>
         <v/>
       </c>
-      <c r="B22" s="300"/>
-      <c r="C22" s="300"/>
+      <c r="B22" s="306"/>
+      <c r="C22" s="306"/>
       <c r="D22" s="126"/>
       <c r="E22" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35843,8 +35795,8 @@
         <f>IF($B23&lt;&gt;"",COUNTA($B$14:$B23),"")</f>
         <v/>
       </c>
-      <c r="B23" s="300"/>
-      <c r="C23" s="300"/>
+      <c r="B23" s="306"/>
+      <c r="C23" s="306"/>
       <c r="D23" s="126"/>
       <c r="E23" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35861,8 +35813,8 @@
         <f>IF($B24&lt;&gt;"",COUNTA($B$14:$B24),"")</f>
         <v/>
       </c>
-      <c r="B24" s="300"/>
-      <c r="C24" s="300"/>
+      <c r="B24" s="306"/>
+      <c r="C24" s="306"/>
       <c r="D24" s="126"/>
       <c r="E24" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35879,8 +35831,8 @@
         <f>IF($B25&lt;&gt;"",COUNTA($B$14:$B25),"")</f>
         <v/>
       </c>
-      <c r="B25" s="300"/>
-      <c r="C25" s="300"/>
+      <c r="B25" s="306"/>
+      <c r="C25" s="306"/>
       <c r="D25" s="126"/>
       <c r="E25" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35897,8 +35849,8 @@
         <f>IF($B26&lt;&gt;"",COUNTA($B$14:$B26),"")</f>
         <v/>
       </c>
-      <c r="B26" s="300"/>
-      <c r="C26" s="300"/>
+      <c r="B26" s="306"/>
+      <c r="C26" s="306"/>
       <c r="D26" s="126"/>
       <c r="E26" s="121" t="str">
         <f t="shared" si="0"/>
@@ -35915,8 +35867,8 @@
         <f>IF($B27&lt;&gt;"",COUNTA($B$14:$B27),"")</f>
         <v/>
       </c>
-      <c r="B27" s="315"/>
-      <c r="C27" s="315"/>
+      <c r="B27" s="321"/>
+      <c r="C27" s="321"/>
       <c r="D27" s="128"/>
       <c r="E27" s="129" t="str">
         <f t="shared" si="0"/>
@@ -35951,12 +35903,12 @@
       <c r="B30" s="64"/>
       <c r="C30" s="97"/>
       <c r="D30" s="132"/>
-      <c r="E30" s="266" t="str">
+      <c r="E30" s="271" t="str">
         <f>"Padang, …................................."</f>
         <v>Padang, ….................................</v>
       </c>
-      <c r="F30" s="266"/>
-      <c r="G30" s="316"/>
+      <c r="F30" s="271"/>
+      <c r="G30" s="322"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="133" t="s">
@@ -35969,7 +35921,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="267"/>
-      <c r="G31" s="317"/>
+      <c r="G31" s="323"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="101"/>
@@ -36005,11 +35957,11 @@
       <c r="B35" s="95"/>
       <c r="C35" s="75"/>
       <c r="D35" s="67"/>
-      <c r="E35" s="262" t="s">
+      <c r="E35" s="265" t="s">
         <v>1138</v>
       </c>
-      <c r="F35" s="262"/>
-      <c r="G35" s="318"/>
+      <c r="F35" s="265"/>
+      <c r="G35" s="324"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="104" t="s">
@@ -36018,12 +35970,12 @@
       <c r="B36" s="134"/>
       <c r="C36" s="76"/>
       <c r="D36" s="134"/>
-      <c r="E36" s="312" t="str">
+      <c r="E36" s="318" t="str">
         <f>_xlfn.XLOOKUP($E35,db_pegawai!$B$2:$B$90,db_pegawai!$I$2:$I$90,"")</f>
         <v/>
       </c>
-      <c r="F36" s="313"/>
-      <c r="G36" s="314"/>
+      <c r="F36" s="319"/>
+      <c r="G36" s="320"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="77" t="s">
@@ -39025,17 +38977,17 @@
       <c r="AA1" s="227"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="319" t="s">
+      <c r="A2" s="325" t="s">
         <v>1189</v>
       </c>
-      <c r="B2" s="320"/>
-      <c r="C2" s="320"/>
-      <c r="D2" s="320"/>
-      <c r="E2" s="320"/>
-      <c r="F2" s="320"/>
-      <c r="G2" s="320"/>
-      <c r="H2" s="320"/>
-      <c r="I2" s="320"/>
+      <c r="B2" s="326"/>
+      <c r="C2" s="326"/>
+      <c r="D2" s="326"/>
+      <c r="E2" s="326"/>
+      <c r="F2" s="326"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="326"/>
       <c r="J2" s="227"/>
       <c r="K2" s="227"/>
       <c r="L2" s="227"/>
@@ -39085,35 +39037,35 @@
       <c r="AA3" s="227"/>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="321" t="s">
+      <c r="A4" s="327" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="322" t="s">
+      <c r="B4" s="328" t="s">
         <v>1190</v>
       </c>
-      <c r="C4" s="322" t="s">
+      <c r="C4" s="328" t="s">
         <v>1191</v>
       </c>
-      <c r="D4" s="324" t="s">
+      <c r="D4" s="330" t="s">
         <v>1192</v>
       </c>
-      <c r="E4" s="326" t="s">
+      <c r="E4" s="332" t="s">
         <v>1193</v>
       </c>
-      <c r="F4" s="327"/>
-      <c r="G4" s="328" t="s">
+      <c r="F4" s="333"/>
+      <c r="G4" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="329" t="s">
+      <c r="H4" s="335" t="s">
         <v>1139</v>
       </c>
-      <c r="I4" s="328" t="s">
+      <c r="I4" s="334" t="s">
         <v>311</v>
       </c>
-      <c r="J4" s="331" t="s">
+      <c r="J4" s="337" t="s">
         <v>1194</v>
       </c>
-      <c r="K4" s="331" t="s">
+      <c r="K4" s="337" t="s">
         <v>272</v>
       </c>
       <c r="L4" s="227"/>
@@ -39134,21 +39086,21 @@
       <c r="AA4" s="227"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="321"/>
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="325"/>
+      <c r="A5" s="327"/>
+      <c r="B5" s="329"/>
+      <c r="C5" s="329"/>
+      <c r="D5" s="331"/>
       <c r="E5" s="208" t="s">
         <v>1195</v>
       </c>
       <c r="F5" s="208" t="s">
         <v>1192</v>
       </c>
-      <c r="G5" s="328"/>
-      <c r="H5" s="329"/>
-      <c r="I5" s="328"/>
-      <c r="J5" s="331"/>
-      <c r="K5" s="331"/>
+      <c r="G5" s="334"/>
+      <c r="H5" s="335"/>
+      <c r="I5" s="334"/>
+      <c r="J5" s="337"/>
+      <c r="K5" s="337"/>
       <c r="L5" s="227"/>
       <c r="M5" s="227"/>
       <c r="N5" s="227"/>
@@ -40417,14 +40369,14 @@
     </row>
     <row r="36" spans="1:11" s="206" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="217"/>
-      <c r="B36" s="332" t="s">
+      <c r="B36" s="338" t="s">
         <v>311</v>
       </c>
-      <c r="C36" s="333"/>
-      <c r="D36" s="334"/>
-      <c r="E36" s="333"/>
-      <c r="F36" s="333"/>
-      <c r="G36" s="335"/>
+      <c r="C36" s="339"/>
+      <c r="D36" s="340"/>
+      <c r="E36" s="339"/>
+      <c r="F36" s="339"/>
+      <c r="G36" s="341"/>
       <c r="H36" s="233"/>
       <c r="I36" s="218">
         <f>SUM(I7:I35)</f>
@@ -40435,17 +40387,17 @@
     </row>
     <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="219"/>
-      <c r="B37" s="336" t="str">
+      <c r="B37" s="342" t="str">
         <f>"Terbilang: "&amp;IF(I36=0,"nol",IF(I36&lt;0,"minus ","")&amp;SUBSTITUTE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(IF(--MID(TEXT(ABS(I36),"000000000000000"),1,3)=0,"",MID(TEXT(ABS(I36),"000000000000000"),1,1)&amp;" ratus "&amp;MID(TEXT(ABS(I36),"000000000000000"),2,1)&amp;" puluh "&amp;MID(TEXT(ABS(I36),"000000000000000"),3,1)&amp;" trilyun ")&amp;IF(--MID(TEXT(ABS(I36),"000000000000000"),4,3)=0,"",MID(TEXT(ABS(I36),"000000000000000"),4,1)&amp;" ratus "&amp;MID(TEXT(ABS(I36),"000000000000000"),5,1)&amp;" puluh "&amp;MID(TEXT(ABS(I36),"000000000000000"),6,1)&amp;" milyar ")&amp;IF(--MID(TEXT(ABS(I36),"000000000000000"),7,3)=0,"",MID(TEXT(ABS(I36),"000000000000000"),7,1)&amp;" ratus "&amp;MID(TEXT(ABS(I36),"000000000000000"),8,1)&amp;" puluh "&amp;MID(TEXT(ABS(I36),"000000000000000"),9,1)&amp;" juta ")&amp;IF(--MID(TEXT(ABS(I36),"000000000000000"),10,3)=0,"",IF(--MID(TEXT(ABS(I36),"000000000000000"),10,3)=1,"*",MID(TEXT(ABS(I36),"000000000000000"),10,1)&amp;" ratus "&amp;MID(TEXT(ABS(I36),"000000000000000"),11,1)&amp;" puluh ")&amp;MID(TEXT(ABS(I36),"000000000000000"),12,1)&amp;" ribu ")&amp;IF(--MID(TEXT(ABS(I36),"000000000000000"),13,3)=0,"",MID(TEXT(ABS(I36),"000000000000000"),13,1)&amp;" ratus "&amp;MID(TEXT(ABS(I36),"000000000000000"),14,1)&amp;" puluh "&amp;MID(TEXT(ABS(I36),"000000000000000"),15,1)),1,"satu"),2,"dua"),3,"tiga"),4,"empat"),5,"lima"),6,"enam"),7,"tujuh"),8,"delapan"),9,"sembilan"),"0 ratus",""),"0 puluh",""),"satu puluh 0","sepuluh"),"satu puluh satu","sebelas"),"satu puluh dua","duabelas"),"satu puluh tiga","tiga belas"),"satu puluh empat","empatbelas"),"satu puluh lima","limabelas"),"satu puluh enam","enambelas"),"satu puluh tujuh","tujuhbelas"),"satu puluh delapan","delapan belas"),"satu puluh sembilan","sembilanbelas"),"satu ratus","seratus"),"*satu ribu","seribu"),0,""))," "," "))&amp;" rupiah"</f>
         <v>Terbilang: delapan belas juta sembilan ratus tiga puluh empat ribu tiga ratus rupiah</v>
       </c>
-      <c r="C37" s="337"/>
-      <c r="D37" s="337"/>
-      <c r="E37" s="337"/>
-      <c r="F37" s="337"/>
-      <c r="G37" s="338"/>
-      <c r="H37" s="337"/>
-      <c r="I37" s="338"/>
+      <c r="C37" s="343"/>
+      <c r="D37" s="343"/>
+      <c r="E37" s="343"/>
+      <c r="F37" s="343"/>
+      <c r="G37" s="344"/>
+      <c r="H37" s="343"/>
+      <c r="I37" s="344"/>
       <c r="J37" s="227"/>
       <c r="K37" s="227"/>
     </row>
@@ -40457,8 +40409,8 @@
       <c r="E38" s="227"/>
       <c r="F38" s="227"/>
       <c r="G38" s="220"/>
-      <c r="H38" s="339"/>
-      <c r="I38" s="339"/>
+      <c r="H38" s="345"/>
+      <c r="I38" s="345"/>
       <c r="J38" s="227"/>
       <c r="K38" s="227"/>
     </row>
@@ -40470,12 +40422,12 @@
       <c r="C39" s="227"/>
       <c r="D39" s="227"/>
       <c r="E39" s="227"/>
-      <c r="F39" s="340" t="e" vm="1">
+      <c r="F39" s="346" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="G39" s="340"/>
-      <c r="H39" s="340"/>
-      <c r="I39" s="340"/>
+      <c r="G39" s="346"/>
+      <c r="H39" s="346"/>
+      <c r="I39" s="346"/>
       <c r="J39" s="227"/>
       <c r="K39" s="227"/>
     </row>
@@ -40487,10 +40439,10 @@
       <c r="C40" s="227"/>
       <c r="D40" s="227"/>
       <c r="E40" s="227"/>
-      <c r="F40" s="340"/>
-      <c r="G40" s="340"/>
-      <c r="H40" s="340"/>
-      <c r="I40" s="340"/>
+      <c r="F40" s="346"/>
+      <c r="G40" s="346"/>
+      <c r="H40" s="346"/>
+      <c r="I40" s="346"/>
       <c r="J40" s="227"/>
       <c r="K40" s="227"/>
     </row>
@@ -40567,12 +40519,12 @@
       <c r="C46" s="227"/>
       <c r="D46" s="227"/>
       <c r="E46" s="227"/>
-      <c r="F46" s="341" t="e" vm="1">
+      <c r="F46" s="347" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="G46" s="341"/>
-      <c r="H46" s="341"/>
-      <c r="I46" s="341"/>
+      <c r="G46" s="347"/>
+      <c r="H46" s="347"/>
+      <c r="I46" s="347"/>
       <c r="J46" s="227"/>
       <c r="K46" s="227"/>
     </row>
@@ -40584,12 +40536,12 @@
       <c r="C47" s="227"/>
       <c r="D47" s="227"/>
       <c r="E47" s="227"/>
-      <c r="F47" s="330" t="e" vm="1">
+      <c r="F47" s="336" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="G47" s="330"/>
-      <c r="H47" s="330"/>
-      <c r="I47" s="330"/>
+      <c r="G47" s="336"/>
+      <c r="H47" s="336"/>
+      <c r="I47" s="336"/>
       <c r="J47" s="227"/>
       <c r="K47" s="227"/>
     </row>
@@ -74336,42 +74288,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="287" t="s">
         <v>611</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="281"/>
-      <c r="M1" s="281"/>
-      <c r="N1" s="281"/>
-      <c r="O1" s="281"/>
-      <c r="P1" s="281"/>
-      <c r="Q1" s="281"/>
-      <c r="R1" s="281"/>
-      <c r="S1" s="281"/>
-      <c r="T1" s="281"/>
-      <c r="U1" s="281"/>
-      <c r="V1" s="281"/>
-      <c r="W1" s="281"/>
-      <c r="X1" s="281"/>
-      <c r="Y1" s="281"/>
-      <c r="Z1" s="281"/>
-      <c r="AA1" s="281"/>
-      <c r="AB1" s="281"/>
-      <c r="AC1" s="281"/>
-      <c r="AD1" s="281"/>
-      <c r="AE1" s="281"/>
-      <c r="AF1" s="281"/>
-      <c r="AG1" s="281"/>
-      <c r="AH1" s="281"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
+      <c r="P1" s="287"/>
+      <c r="Q1" s="287"/>
+      <c r="R1" s="287"/>
+      <c r="S1" s="287"/>
+      <c r="T1" s="287"/>
+      <c r="U1" s="287"/>
+      <c r="V1" s="287"/>
+      <c r="W1" s="287"/>
+      <c r="X1" s="287"/>
+      <c r="Y1" s="287"/>
+      <c r="Z1" s="287"/>
+      <c r="AA1" s="287"/>
+      <c r="AB1" s="287"/>
+      <c r="AC1" s="287"/>
+      <c r="AD1" s="287"/>
+      <c r="AE1" s="287"/>
+      <c r="AF1" s="287"/>
+      <c r="AG1" s="287"/>
+      <c r="AH1" s="287"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AA2" s="138" t="s">
@@ -74404,17 +74356,17 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="282" t="s">
+      <c r="A4" s="288" t="s">
         <v>617</v>
       </c>
-      <c r="B4" s="282"/>
-      <c r="C4" s="282"/>
-      <c r="D4" s="282"/>
-      <c r="E4" s="282"/>
-      <c r="F4" s="282"/>
-      <c r="G4" s="282"/>
-      <c r="H4" s="282"/>
-      <c r="I4" s="282"/>
+      <c r="B4" s="288"/>
+      <c r="C4" s="288"/>
+      <c r="D4" s="288"/>
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288"/>
+      <c r="H4" s="288"/>
+      <c r="I4" s="288"/>
       <c r="L4" s="138" t="s">
         <v>618</v>
       </c>
@@ -74451,48 +74403,48 @@
     </row>
     <row r="6" spans="1:34" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="283" t="s">
+      <c r="A7" s="289" t="s">
         <v>623</v>
       </c>
-      <c r="B7" s="284"/>
-      <c r="C7" s="284"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="284"/>
-      <c r="H7" s="284"/>
-      <c r="I7" s="284"/>
-      <c r="J7" s="284"/>
-      <c r="K7" s="284"/>
-      <c r="L7" s="284"/>
-      <c r="M7" s="284"/>
-      <c r="N7" s="284"/>
-      <c r="O7" s="284"/>
-      <c r="P7" s="284"/>
-      <c r="Q7" s="284"/>
-      <c r="R7" s="284"/>
-      <c r="S7" s="284"/>
-      <c r="T7" s="284"/>
-      <c r="U7" s="284"/>
-      <c r="V7" s="284"/>
-      <c r="W7" s="284"/>
-      <c r="X7" s="285"/>
-      <c r="Y7" s="290" t="s">
+      <c r="B7" s="290"/>
+      <c r="C7" s="290"/>
+      <c r="D7" s="290"/>
+      <c r="E7" s="290"/>
+      <c r="F7" s="290"/>
+      <c r="G7" s="290"/>
+      <c r="H7" s="290"/>
+      <c r="I7" s="290"/>
+      <c r="J7" s="290"/>
+      <c r="K7" s="290"/>
+      <c r="L7" s="290"/>
+      <c r="M7" s="290"/>
+      <c r="N7" s="290"/>
+      <c r="O7" s="290"/>
+      <c r="P7" s="290"/>
+      <c r="Q7" s="290"/>
+      <c r="R7" s="290"/>
+      <c r="S7" s="290"/>
+      <c r="T7" s="290"/>
+      <c r="U7" s="290"/>
+      <c r="V7" s="290"/>
+      <c r="W7" s="290"/>
+      <c r="X7" s="291"/>
+      <c r="Y7" s="296" t="s">
         <v>624</v>
       </c>
-      <c r="Z7" s="291"/>
-      <c r="AA7" s="292"/>
-      <c r="AB7" s="290" t="s">
+      <c r="Z7" s="297"/>
+      <c r="AA7" s="298"/>
+      <c r="AB7" s="296" t="s">
         <v>625</v>
       </c>
-      <c r="AC7" s="291"/>
-      <c r="AD7" s="292"/>
-      <c r="AE7" s="286" t="s">
+      <c r="AC7" s="297"/>
+      <c r="AD7" s="298"/>
+      <c r="AE7" s="292" t="s">
         <v>626</v>
       </c>
-      <c r="AF7" s="287"/>
-      <c r="AG7" s="287"/>
-      <c r="AH7" s="288"/>
+      <c r="AF7" s="293"/>
+      <c r="AG7" s="293"/>
+      <c r="AH7" s="294"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="140"/>
@@ -74519,16 +74471,16 @@
       <c r="V8" s="247"/>
       <c r="W8" s="248"/>
       <c r="X8" s="247"/>
-      <c r="Y8" s="293"/>
-      <c r="Z8" s="294"/>
-      <c r="AA8" s="295"/>
-      <c r="AB8" s="293"/>
-      <c r="AC8" s="294"/>
-      <c r="AD8" s="295"/>
-      <c r="AE8" s="274"/>
-      <c r="AF8" s="280"/>
-      <c r="AG8" s="280"/>
-      <c r="AH8" s="279"/>
+      <c r="Y8" s="299"/>
+      <c r="Z8" s="300"/>
+      <c r="AA8" s="301"/>
+      <c r="AB8" s="299"/>
+      <c r="AC8" s="300"/>
+      <c r="AD8" s="301"/>
+      <c r="AE8" s="280"/>
+      <c r="AF8" s="286"/>
+      <c r="AG8" s="286"/>
+      <c r="AH8" s="285"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="141" t="s">
@@ -74579,16 +74531,16 @@
         <v>638</v>
       </c>
       <c r="X9" s="142"/>
-      <c r="Y9" s="296"/>
-      <c r="Z9" s="297"/>
-      <c r="AA9" s="298"/>
-      <c r="AB9" s="296"/>
-      <c r="AC9" s="297"/>
-      <c r="AD9" s="298"/>
-      <c r="AE9" s="271"/>
-      <c r="AF9" s="289"/>
-      <c r="AG9" s="289"/>
-      <c r="AH9" s="276"/>
+      <c r="Y9" s="302"/>
+      <c r="Z9" s="303"/>
+      <c r="AA9" s="304"/>
+      <c r="AB9" s="302"/>
+      <c r="AC9" s="303"/>
+      <c r="AD9" s="304"/>
+      <c r="AE9" s="277"/>
+      <c r="AF9" s="295"/>
+      <c r="AG9" s="295"/>
+      <c r="AH9" s="282"/>
     </row>
     <row r="10" spans="1:34" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="144" t="s">
@@ -74665,10 +74617,10 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="152"/>
-      <c r="B12" s="286" t="s">
+      <c r="B12" s="292" t="s">
         <v>644</v>
       </c>
-      <c r="C12" s="288"/>
+      <c r="C12" s="294"/>
       <c r="D12" s="153"/>
       <c r="E12" s="154"/>
       <c r="F12" s="153"/>
@@ -74684,10 +74636,10 @@
       <c r="P12" s="153"/>
       <c r="Q12" s="154"/>
       <c r="R12" s="155"/>
-      <c r="S12" s="286" t="s">
+      <c r="S12" s="292" t="s">
         <v>644</v>
       </c>
-      <c r="T12" s="288"/>
+      <c r="T12" s="294"/>
       <c r="U12" s="153"/>
       <c r="V12" s="154"/>
       <c r="W12" s="153"/>
@@ -74707,185 +74659,185 @@
       <c r="A13" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="274" t="s">
+      <c r="B13" s="280" t="s">
         <v>645</v>
       </c>
-      <c r="C13" s="279"/>
-      <c r="D13" s="274" t="s">
+      <c r="C13" s="285"/>
+      <c r="D13" s="280" t="s">
         <v>646</v>
       </c>
-      <c r="E13" s="279"/>
-      <c r="F13" s="274" t="s">
+      <c r="E13" s="285"/>
+      <c r="F13" s="280" t="s">
         <v>647</v>
       </c>
-      <c r="G13" s="280"/>
-      <c r="H13" s="280"/>
-      <c r="I13" s="280"/>
-      <c r="J13" s="280"/>
-      <c r="K13" s="279"/>
-      <c r="L13" s="274" t="s">
+      <c r="G13" s="286"/>
+      <c r="H13" s="286"/>
+      <c r="I13" s="286"/>
+      <c r="J13" s="286"/>
+      <c r="K13" s="285"/>
+      <c r="L13" s="280" t="s">
         <v>648</v>
       </c>
-      <c r="M13" s="279"/>
-      <c r="N13" s="274" t="s">
+      <c r="M13" s="285"/>
+      <c r="N13" s="280" t="s">
         <v>649</v>
       </c>
-      <c r="O13" s="279"/>
-      <c r="P13" s="274" t="s">
+      <c r="O13" s="285"/>
+      <c r="P13" s="280" t="s">
         <v>650</v>
       </c>
-      <c r="Q13" s="279"/>
+      <c r="Q13" s="285"/>
       <c r="R13" s="158" t="s">
         <v>644</v>
       </c>
-      <c r="S13" s="274" t="s">
+      <c r="S13" s="280" t="s">
         <v>645</v>
       </c>
-      <c r="T13" s="279"/>
-      <c r="U13" s="274" t="s">
+      <c r="T13" s="285"/>
+      <c r="U13" s="280" t="s">
         <v>646</v>
       </c>
-      <c r="V13" s="279"/>
-      <c r="W13" s="274" t="s">
+      <c r="V13" s="285"/>
+      <c r="W13" s="280" t="s">
         <v>647</v>
       </c>
-      <c r="X13" s="280"/>
-      <c r="Y13" s="280"/>
-      <c r="Z13" s="280"/>
-      <c r="AA13" s="280"/>
-      <c r="AB13" s="279"/>
-      <c r="AC13" s="274" t="s">
+      <c r="X13" s="286"/>
+      <c r="Y13" s="286"/>
+      <c r="Z13" s="286"/>
+      <c r="AA13" s="286"/>
+      <c r="AB13" s="285"/>
+      <c r="AC13" s="280" t="s">
         <v>648</v>
       </c>
-      <c r="AD13" s="279"/>
-      <c r="AE13" s="274" t="s">
+      <c r="AD13" s="285"/>
+      <c r="AE13" s="280" t="s">
         <v>649</v>
       </c>
-      <c r="AF13" s="279"/>
-      <c r="AG13" s="274" t="s">
+      <c r="AF13" s="285"/>
+      <c r="AG13" s="280" t="s">
         <v>650</v>
       </c>
-      <c r="AH13" s="275"/>
+      <c r="AH13" s="281"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="159"/>
-      <c r="B14" s="271" t="s">
+      <c r="B14" s="277" t="s">
         <v>651</v>
       </c>
-      <c r="C14" s="276"/>
-      <c r="D14" s="271" t="s">
+      <c r="C14" s="282"/>
+      <c r="D14" s="277" t="s">
         <v>652</v>
       </c>
-      <c r="E14" s="276"/>
+      <c r="E14" s="282"/>
       <c r="F14" s="143"/>
       <c r="G14" s="143"/>
       <c r="H14" s="143"/>
       <c r="I14" s="143"/>
       <c r="J14" s="143"/>
       <c r="K14" s="142"/>
-      <c r="L14" s="277" t="s">
+      <c r="L14" s="283" t="s">
         <v>653</v>
       </c>
-      <c r="M14" s="278"/>
-      <c r="N14" s="277" t="s">
+      <c r="M14" s="284"/>
+      <c r="N14" s="283" t="s">
         <v>654</v>
       </c>
-      <c r="O14" s="278"/>
-      <c r="P14" s="271" t="s">
+      <c r="O14" s="284"/>
+      <c r="P14" s="277" t="s">
         <v>655</v>
       </c>
-      <c r="Q14" s="276"/>
+      <c r="Q14" s="282"/>
       <c r="R14" s="159"/>
-      <c r="S14" s="271" t="s">
+      <c r="S14" s="277" t="s">
         <v>651</v>
       </c>
-      <c r="T14" s="276"/>
-      <c r="U14" s="271" t="s">
+      <c r="T14" s="282"/>
+      <c r="U14" s="277" t="s">
         <v>652</v>
       </c>
-      <c r="V14" s="276"/>
+      <c r="V14" s="282"/>
       <c r="W14" s="143"/>
       <c r="X14" s="143"/>
       <c r="Y14" s="143"/>
       <c r="Z14" s="143"/>
       <c r="AA14" s="143"/>
       <c r="AB14" s="142"/>
-      <c r="AC14" s="277" t="s">
+      <c r="AC14" s="283" t="s">
         <v>653</v>
       </c>
-      <c r="AD14" s="278"/>
-      <c r="AE14" s="277" t="s">
+      <c r="AD14" s="284"/>
+      <c r="AE14" s="283" t="s">
         <v>654</v>
       </c>
-      <c r="AF14" s="278"/>
-      <c r="AG14" s="271" t="s">
+      <c r="AF14" s="284"/>
+      <c r="AG14" s="277" t="s">
         <v>655</v>
       </c>
-      <c r="AH14" s="272"/>
+      <c r="AH14" s="278"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="160" t="s">
         <v>656</v>
       </c>
-      <c r="B15" s="268" t="s">
+      <c r="B15" s="274" t="s">
         <v>657</v>
       </c>
-      <c r="C15" s="269"/>
-      <c r="D15" s="268" t="s">
+      <c r="C15" s="275"/>
+      <c r="D15" s="274" t="s">
         <v>658</v>
       </c>
-      <c r="E15" s="269"/>
-      <c r="F15" s="268" t="s">
+      <c r="E15" s="275"/>
+      <c r="F15" s="274" t="s">
         <v>659</v>
       </c>
-      <c r="G15" s="273"/>
-      <c r="H15" s="273"/>
-      <c r="I15" s="273"/>
-      <c r="J15" s="273"/>
-      <c r="K15" s="269"/>
-      <c r="L15" s="268" t="s">
+      <c r="G15" s="279"/>
+      <c r="H15" s="279"/>
+      <c r="I15" s="279"/>
+      <c r="J15" s="279"/>
+      <c r="K15" s="275"/>
+      <c r="L15" s="274" t="s">
         <v>660</v>
       </c>
-      <c r="M15" s="269"/>
-      <c r="N15" s="268" t="s">
+      <c r="M15" s="275"/>
+      <c r="N15" s="274" t="s">
         <v>661</v>
       </c>
-      <c r="O15" s="269"/>
-      <c r="P15" s="268" t="s">
+      <c r="O15" s="275"/>
+      <c r="P15" s="274" t="s">
         <v>662</v>
       </c>
-      <c r="Q15" s="270"/>
+      <c r="Q15" s="276"/>
       <c r="R15" s="160" t="s">
         <v>656</v>
       </c>
-      <c r="S15" s="268" t="s">
+      <c r="S15" s="274" t="s">
         <v>657</v>
       </c>
-      <c r="T15" s="269"/>
-      <c r="U15" s="268" t="s">
+      <c r="T15" s="275"/>
+      <c r="U15" s="274" t="s">
         <v>658</v>
       </c>
-      <c r="V15" s="269"/>
-      <c r="W15" s="268" t="s">
+      <c r="V15" s="275"/>
+      <c r="W15" s="274" t="s">
         <v>659</v>
       </c>
-      <c r="X15" s="273"/>
-      <c r="Y15" s="273"/>
-      <c r="Z15" s="273"/>
-      <c r="AA15" s="273"/>
-      <c r="AB15" s="269"/>
-      <c r="AC15" s="268" t="s">
+      <c r="X15" s="279"/>
+      <c r="Y15" s="279"/>
+      <c r="Z15" s="279"/>
+      <c r="AA15" s="279"/>
+      <c r="AB15" s="275"/>
+      <c r="AC15" s="274" t="s">
         <v>660</v>
       </c>
-      <c r="AD15" s="269"/>
-      <c r="AE15" s="268" t="s">
+      <c r="AD15" s="275"/>
+      <c r="AE15" s="274" t="s">
         <v>661</v>
       </c>
-      <c r="AF15" s="269"/>
-      <c r="AG15" s="268" t="s">
+      <c r="AF15" s="275"/>
+      <c r="AG15" s="274" t="s">
         <v>662</v>
       </c>
-      <c r="AH15" s="270"/>
+      <c r="AH15" s="276"/>
     </row>
     <row r="16" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="161">
@@ -79733,11 +79685,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="299" t="s">
+      <c r="A1" s="305" t="s">
         <v>1093</v>
       </c>
-      <c r="B1" s="299"/>
-      <c r="C1" s="299"/>
+      <c r="B1" s="305"/>
+      <c r="C1" s="305"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">

</xml_diff>